<commit_message>
Updated contract year and logo, added/removed subs from table
</commit_message>
<xml_diff>
--- a/content/sbs_tef.xlsx
+++ b/content/sbs_tef.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\chc-site\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcollins17\Desktop\github\chc-site\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B0DFF1-1282-41C6-B260-B0A51691E6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC23F0F4-7116-42EA-8915-34D69A231291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34500" yWindow="2070" windowWidth="21600" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -38,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Community Action Agency of Butte County, Inc.</t>
   </si>
@@ -79,9 +92,6 @@
     <t>Napa Valley Community College District </t>
   </si>
   <si>
-    <t>Palo Verde College </t>
-  </si>
-  <si>
     <t>San Luis Obispo, Cal Poly Corporation </t>
   </si>
   <si>
@@ -97,9 +107,6 @@
     <t>University Enterprise, Inc., on behalf of CSU Sacramento </t>
   </si>
   <si>
-    <t>Pitzer College</t>
-  </si>
-  <si>
     <t>The Regents of the University of California, Riverside</t>
   </si>
   <si>
@@ -118,9 +125,6 @@
     <t>San Francisco State University</t>
   </si>
   <si>
-    <t>Sonoma County Community College District (Santa Rosa Junior College)</t>
-  </si>
-  <si>
     <t>The Regents of the University of California, San Diego</t>
   </si>
   <si>
@@ -142,18 +146,12 @@
     <t>BGCC</t>
   </si>
   <si>
-    <t>CSUP</t>
-  </si>
-  <si>
     <t>CSULA</t>
   </si>
   <si>
     <t>CSUDH</t>
   </si>
   <si>
-    <t>CSUB</t>
-  </si>
-  <si>
     <t>CSULB</t>
   </si>
   <si>
@@ -184,9 +182,6 @@
     <t>ELCC</t>
   </si>
   <si>
-    <t>EVCC</t>
-  </si>
-  <si>
     <t>LAMCC</t>
   </si>
   <si>
@@ -202,18 +197,9 @@
     <t>NVCC</t>
   </si>
   <si>
-    <t>PVCC</t>
-  </si>
-  <si>
-    <t>CSUSF</t>
-  </si>
-  <si>
     <t>SLO</t>
   </si>
   <si>
-    <t>SRJC</t>
-  </si>
-  <si>
     <t>CSUSon</t>
   </si>
   <si>
@@ -235,12 +221,6 @@
     <t>Sac</t>
   </si>
   <si>
-    <t>YCC</t>
-  </si>
-  <si>
-    <t>Pitzer</t>
-  </si>
-  <si>
     <t>UCR</t>
   </si>
   <si>
@@ -262,9 +242,6 @@
     <t xml:space="preserve">Cal Poly Pomona Foundation, Inc. </t>
   </si>
   <si>
-    <t xml:space="preserve">California State University Bakersfield, Auxiliary for Sponsored Programs </t>
-  </si>
-  <si>
     <t xml:space="preserve">California State University , Dominguez Hills Foundation </t>
   </si>
   <si>
@@ -280,9 +257,6 @@
     <t>CHABOT</t>
   </si>
   <si>
-    <t xml:space="preserve">Evergreen Valley College </t>
-  </si>
-  <si>
     <t xml:space="preserve">Los Angeles Mission College </t>
   </si>
   <si>
@@ -292,12 +266,6 @@
     <t>PCC</t>
   </si>
   <si>
-    <t>Porterville College</t>
-  </si>
-  <si>
-    <t>Porter</t>
-  </si>
-  <si>
     <t>Rio Hondo Community College District</t>
   </si>
   <si>
@@ -325,12 +293,6 @@
     <t>SMC</t>
   </si>
   <si>
-    <t>Sierra Joint Community College District</t>
-  </si>
-  <si>
-    <t>SIERRA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonoma State University </t>
   </si>
   <si>
@@ -355,19 +317,64 @@
     <t>UCSC</t>
   </si>
   <si>
-    <t>Yuba Community College District (Woodland Community College)</t>
-  </si>
-  <si>
-    <t>WCC</t>
-  </si>
-  <si>
-    <t>Yuba Community College District (Yuba College)</t>
-  </si>
-  <si>
     <t>Campus</t>
   </si>
   <si>
     <t>Shortcode</t>
+  </si>
+  <si>
+    <t>CPP</t>
+  </si>
+  <si>
+    <t>SFSU</t>
+  </si>
+  <si>
+    <t>The Regents of the University of California, Irvine</t>
+  </si>
+  <si>
+    <t>UCI</t>
+  </si>
+  <si>
+    <t>Clovis Community College</t>
+  </si>
+  <si>
+    <t>CLOVIS</t>
+  </si>
+  <si>
+    <t>Compton College</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>LA Valley College</t>
+  </si>
+  <si>
+    <t>LAVC</t>
+  </si>
+  <si>
+    <t>University of California Office of the President</t>
+  </si>
+  <si>
+    <t>UCOP</t>
+  </si>
+  <si>
+    <t>San Diego City College</t>
+  </si>
+  <si>
+    <t>SDCC</t>
+  </si>
+  <si>
+    <t>Irvine Valley College</t>
+  </si>
+  <si>
+    <t>IVC</t>
+  </si>
+  <si>
+    <t>Sutter County Children &amp; Families Commission</t>
+  </si>
+  <si>
+    <t>SutterK</t>
   </si>
 </sst>
 </file>
@@ -435,9 +442,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -475,7 +482,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -581,7 +588,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -723,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,456 +746,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>80</v>
       </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>101</v>
-      </c>
-      <c r="B46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHC site URL and changed table header
</commit_message>
<xml_diff>
--- a/content/sbs_tef.xlsx
+++ b/content/sbs_tef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcollins17\Desktop\github\chc-site\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC23F0F4-7116-42EA-8915-34D69A231291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C5D31E-4D5F-437E-A724-9C9BC550EDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3864" yWindow="0" windowWidth="14832" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,9 +317,6 @@
     <t>UCSC</t>
   </si>
   <si>
-    <t>Campus</t>
-  </si>
-  <si>
     <t>Shortcode</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>SutterK</t>
+  </si>
+  <si>
+    <t>Entity</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -758,10 +760,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,7 +843,7 @@
         <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -910,10 +912,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
         <v>94</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -926,10 +928,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
         <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -950,10 +952,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
         <v>104</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -966,10 +968,10 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
         <v>98</v>
-      </c>
-      <c r="B27" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1033,7 +1035,7 @@
         <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1062,10 +1064,10 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
         <v>102</v>
-      </c>
-      <c r="B39" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1078,10 +1080,10 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
         <v>106</v>
-      </c>
-      <c r="B41" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1102,10 +1104,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
         <v>92</v>
-      </c>
-      <c r="B44" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1158,10 +1160,10 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
         <v>100</v>
-      </c>
-      <c r="B51" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>